<commit_message>
add support for tracking out-of-workspace editing operations through resource change listeners
</commit_message>
<xml_diff>
--- a/emfxcel/net.istvanrath.emfxcel.incquery/samples/demo.xlsx
+++ b/emfxcel/net.istvanrath.emfxcel.incquery/samples/demo.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>képzéskód</t>
   </si>
@@ -52,94 +52,100 @@
     <t>Rendszertervezés</t>
   </si>
   <si>
+    <t>Előtag</t>
+  </si>
+  <si>
+    <t>Név</t>
+  </si>
+  <si>
+    <t>Neptun kód</t>
+  </si>
+  <si>
+    <t>Képzés</t>
+  </si>
+  <si>
+    <t>Évfolyam</t>
+  </si>
+  <si>
+    <t>Felvételek száma</t>
+  </si>
+  <si>
+    <t>Felvett tárgy kódja</t>
+  </si>
+  <si>
+    <t>Felvett tárgy neve</t>
+  </si>
+  <si>
+    <t>Tanrend típus</t>
+  </si>
+  <si>
+    <t>Kurzusra jelentkezett</t>
+  </si>
+  <si>
+    <t>Vizsgára jelentkezhet</t>
+  </si>
+  <si>
+    <t>Várólista</t>
+  </si>
+  <si>
+    <t>Utolsó félév</t>
+  </si>
+  <si>
+    <t>Mérnök informatikus szak, alapképzés</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>BMEVIMIA376</t>
+  </si>
+  <si>
+    <t>Önálló laboratórium</t>
+  </si>
+  <si>
+    <t>2014.02.06. 16:40:26</t>
+  </si>
+  <si>
+    <t>Igen</t>
+  </si>
+  <si>
+    <t>Nem</t>
+  </si>
+  <si>
+    <t>2014.02.03. 16:02:17</t>
+  </si>
+  <si>
+    <t>2014.02.03. 17:07:04</t>
+  </si>
+  <si>
+    <t>Aba Sámuel</t>
+  </si>
+  <si>
+    <t>Szent István</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
+  </si>
+  <si>
+    <t>BCDEFG</t>
+  </si>
+  <si>
+    <t>CDEFGH</t>
+  </si>
+  <si>
+    <t>Gipsz Jakab</t>
+  </si>
+  <si>
+    <t>XYZW99</t>
+  </si>
+  <si>
+    <t>Kasza Elemér</t>
+  </si>
+  <si>
+    <t>DEFGHI</t>
+  </si>
+  <si>
     <t>Nagy Lajos</t>
-  </si>
-  <si>
-    <t>Előtag</t>
-  </si>
-  <si>
-    <t>Név</t>
-  </si>
-  <si>
-    <t>Neptun kód</t>
-  </si>
-  <si>
-    <t>Képzés</t>
-  </si>
-  <si>
-    <t>Évfolyam</t>
-  </si>
-  <si>
-    <t>Felvételek száma</t>
-  </si>
-  <si>
-    <t>Felvett tárgy kódja</t>
-  </si>
-  <si>
-    <t>Felvett tárgy neve</t>
-  </si>
-  <si>
-    <t>Tanrend típus</t>
-  </si>
-  <si>
-    <t>Kurzusra jelentkezett</t>
-  </si>
-  <si>
-    <t>Vizsgára jelentkezhet</t>
-  </si>
-  <si>
-    <t>Várólista</t>
-  </si>
-  <si>
-    <t>Utolsó félév</t>
-  </si>
-  <si>
-    <t>Mérnök informatikus szak, alapképzés</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>BMEVIMIA376</t>
-  </si>
-  <si>
-    <t>Önálló laboratórium</t>
-  </si>
-  <si>
-    <t>2014.02.06. 16:40:26</t>
-  </si>
-  <si>
-    <t>Igen</t>
-  </si>
-  <si>
-    <t>Nem</t>
-  </si>
-  <si>
-    <t>2014.02.03. 16:02:17</t>
-  </si>
-  <si>
-    <t>2014.02.03. 17:07:04</t>
-  </si>
-  <si>
-    <t>Aba Sámuel</t>
-  </si>
-  <si>
-    <t>Szent István</t>
-  </si>
-  <si>
-    <t>ABCDEF</t>
-  </si>
-  <si>
-    <t>BCDEFG</t>
-  </si>
-  <si>
-    <t>CDEFGH</t>
-  </si>
-  <si>
-    <t>Gipsz Jakab</t>
-  </si>
-  <si>
-    <t>XYZW99</t>
   </si>
 </sst>
 </file>
@@ -233,9 +239,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -260,17 +268,19 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -669,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:F4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -702,10 +712,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -722,10 +732,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -742,10 +752,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -754,6 +764,26 @@
         <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -797,43 +827,43 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -848,36 +878,36 @@
     <row r="2" spans="1:22">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="M2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -894,36 +924,36 @@
     <row r="3" spans="1:22">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="M3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -940,36 +970,36 @@
     <row r="4" spans="1:22">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="M4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>

</xml_diff>